<commit_message>
Add new solution for creating new clean spreadsheet instead of removing duplicates from original
</commit_message>
<xml_diff>
--- a/test-headers.xlsx
+++ b/test-headers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>account</t>
   </si>
@@ -46,24 +46,6 @@
     <t>hdhdhd</t>
   </si>
   <si>
-    <t>fhfef</t>
-  </si>
-  <si>
-    <t>sjdjjdjk</t>
-  </si>
-  <si>
-    <t>jekekf</t>
-  </si>
-  <si>
-    <t>sjsjdjjde</t>
-  </si>
-  <si>
-    <t>jdjjfjee</t>
-  </si>
-  <si>
-    <t>ddeeue</t>
-  </si>
-  <si>
     <t>djdjjdd</t>
   </si>
   <si>
@@ -80,24 +62,6 @@
   </si>
   <si>
     <t>grr</t>
-  </si>
-  <si>
-    <t>esskkf</t>
-  </si>
-  <si>
-    <t>ee</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
-    <t>jddkd</t>
-  </si>
-  <si>
-    <t>dddkkd</t>
-  </si>
-  <si>
-    <t>fiirir</t>
   </si>
 </sst>
 </file>
@@ -455,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -480,7 +444,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -491,7 +455,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -502,7 +466,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -513,7 +477,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -524,7 +488,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -535,7 +499,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -546,73 +510,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>501</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>502</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>503</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>504</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>505</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>506</v>
-      </c>
-      <c r="B14" t="s">
         <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>